<commit_message>
Task description files added
</commit_message>
<xml_diff>
--- a/adult_trog/adult_trog_task.xlsx
+++ b/adult_trog/adult_trog_task.xlsx
@@ -1487,621 +1487,621 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="F3" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="G3" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="H3" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="I3" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>57</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>58</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>59</v>
       </c>
       <c r="G4" t="s">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="H4" t="s">
-        <v>16</v>
+        <v>61</v>
       </c>
       <c r="I4" t="s">
-        <v>15</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>62</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>63</v>
       </c>
       <c r="F5" t="s">
-        <v>19</v>
+        <v>64</v>
       </c>
       <c r="G5" t="s">
-        <v>20</v>
+        <v>65</v>
       </c>
       <c r="H5" t="s">
-        <v>21</v>
+        <v>66</v>
       </c>
       <c r="I5" t="s">
-        <v>20</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E6" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="F6" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="G6" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="H6" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="I6" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>27</v>
+        <v>67</v>
       </c>
       <c r="E7" t="s">
-        <v>28</v>
+        <v>68</v>
       </c>
       <c r="F7" t="s">
-        <v>29</v>
+        <v>69</v>
       </c>
       <c r="G7" t="s">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="H7" t="s">
-        <v>31</v>
+        <v>71</v>
       </c>
       <c r="I7" t="s">
-        <v>29</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="F8" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="G8" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="H8" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="I8" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="E9" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="F9" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="G9" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="H9" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="I9" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E10" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="F10" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="G10" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="H10" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="I10" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
       <c r="E11" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="F11" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="G11" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="H11" t="s">
-        <v>51</v>
+        <v>16</v>
       </c>
       <c r="I11" t="s">
-        <v>51</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="E12" t="s">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="F12" t="s">
-        <v>54</v>
+        <v>19</v>
       </c>
       <c r="G12" t="s">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="H12" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="I12" t="s">
-        <v>56</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="E13" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="F13" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="G13" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="H13" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="I13" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="E14" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="F14" t="s">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="G14" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
       <c r="H14" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="I14" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>67</v>
+        <v>22</v>
       </c>
       <c r="E15" t="s">
-        <v>68</v>
+        <v>23</v>
       </c>
       <c r="F15" t="s">
-        <v>69</v>
+        <v>24</v>
       </c>
       <c r="G15" t="s">
-        <v>70</v>
+        <v>25</v>
       </c>
       <c r="H15" t="s">
-        <v>71</v>
+        <v>26</v>
       </c>
       <c r="I15" t="s">
-        <v>69</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="E16" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="F16" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="G16" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="H16" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="I16" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="E17" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="F17" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="G17" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="H17" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="I17" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>82</v>
+        <v>52</v>
       </c>
       <c r="E18" t="s">
-        <v>83</v>
+        <v>53</v>
       </c>
       <c r="F18" t="s">
-        <v>84</v>
+        <v>54</v>
       </c>
       <c r="G18" t="s">
-        <v>85</v>
+        <v>55</v>
       </c>
       <c r="H18" t="s">
-        <v>86</v>
+        <v>56</v>
       </c>
       <c r="I18" t="s">
-        <v>86</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="B19" t="s">
         <v>87</v>
       </c>
       <c r="C19" t="s">
-        <v>88</v>
+        <v>118</v>
       </c>
       <c r="D19" t="s">
-        <v>89</v>
+        <v>170</v>
       </c>
       <c r="E19" t="s">
-        <v>90</v>
+        <v>171</v>
       </c>
       <c r="F19" t="s">
-        <v>91</v>
+        <v>172</v>
       </c>
       <c r="G19" t="s">
-        <v>92</v>
+        <v>173</v>
       </c>
       <c r="H19" t="s">
-        <v>93</v>
+        <v>174</v>
       </c>
       <c r="I19" t="s">
-        <v>90</v>
+        <v>174</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="B20" t="s">
         <v>87</v>
       </c>
       <c r="C20" t="s">
-        <v>94</v>
+        <v>118</v>
       </c>
       <c r="D20" t="s">
-        <v>95</v>
+        <v>119</v>
       </c>
       <c r="E20" t="s">
-        <v>96</v>
+        <v>120</v>
       </c>
       <c r="F20" t="s">
-        <v>97</v>
+        <v>121</v>
       </c>
       <c r="G20" t="s">
-        <v>98</v>
+        <v>122</v>
       </c>
       <c r="H20" t="s">
-        <v>99</v>
+        <v>123</v>
       </c>
       <c r="I20" t="s">
-        <v>99</v>
+        <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="B21" t="s">
         <v>87</v>
       </c>
       <c r="C21" t="s">
-        <v>100</v>
+        <v>124</v>
       </c>
       <c r="D21" t="s">
-        <v>101</v>
+        <v>160</v>
       </c>
       <c r="E21" t="s">
-        <v>102</v>
+        <v>161</v>
       </c>
       <c r="F21" t="s">
-        <v>103</v>
+        <v>162</v>
       </c>
       <c r="G21" t="s">
-        <v>104</v>
+        <v>163</v>
       </c>
       <c r="H21" t="s">
-        <v>105</v>
+        <v>164</v>
       </c>
       <c r="I21" t="s">
-        <v>102</v>
+        <v>164</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B22" t="s">
         <v>87</v>
       </c>
       <c r="C22" t="s">
-        <v>106</v>
+        <v>124</v>
       </c>
       <c r="D22" t="s">
-        <v>107</v>
+        <v>165</v>
       </c>
       <c r="E22" t="s">
-        <v>108</v>
+        <v>166</v>
       </c>
       <c r="F22" t="s">
-        <v>109</v>
+        <v>167</v>
       </c>
       <c r="G22" t="s">
-        <v>110</v>
+        <v>168</v>
       </c>
       <c r="H22" t="s">
-        <v>111</v>
+        <v>169</v>
       </c>
       <c r="I22" t="s">
-        <v>109</v>
+        <v>167</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B23" t="s">
         <v>87</v>
       </c>
       <c r="C23" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="D23" t="s">
-        <v>113</v>
+        <v>150</v>
       </c>
       <c r="E23" t="s">
-        <v>114</v>
+        <v>151</v>
       </c>
       <c r="F23" t="s">
-        <v>115</v>
+        <v>152</v>
       </c>
       <c r="G23" t="s">
-        <v>116</v>
+        <v>153</v>
       </c>
       <c r="H23" t="s">
-        <v>117</v>
+        <v>154</v>
       </c>
       <c r="I23" t="s">
-        <v>114</v>
+        <v>153</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B24" t="s">
         <v>87</v>
       </c>
       <c r="C24" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="D24" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="E24" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="F24" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="G24" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="H24" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="I24" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B25" t="s">
         <v>87</v>
       </c>
       <c r="C25" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="D25" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="E25" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="F25" t="s">
-        <v>127</v>
+        <v>137</v>
       </c>
       <c r="G25" t="s">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="H25" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
       <c r="I25" t="s">
-        <v>126</v>
+        <v>139</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
@@ -2135,7 +2135,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B27" t="s">
         <v>87</v>
@@ -2144,109 +2144,109 @@
         <v>112</v>
       </c>
       <c r="D27" t="s">
-        <v>135</v>
+        <v>113</v>
       </c>
       <c r="E27" t="s">
-        <v>136</v>
+        <v>114</v>
       </c>
       <c r="F27" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="G27" t="s">
-        <v>138</v>
+        <v>116</v>
       </c>
       <c r="H27" t="s">
-        <v>139</v>
+        <v>117</v>
       </c>
       <c r="I27" t="s">
-        <v>139</v>
+        <v>114</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B28" t="s">
         <v>87</v>
       </c>
       <c r="C28" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="D28" t="s">
-        <v>140</v>
+        <v>180</v>
       </c>
       <c r="E28" t="s">
-        <v>141</v>
+        <v>181</v>
       </c>
       <c r="F28" t="s">
-        <v>142</v>
+        <v>182</v>
       </c>
       <c r="G28" t="s">
-        <v>143</v>
+        <v>183</v>
       </c>
       <c r="H28" t="s">
-        <v>144</v>
+        <v>184</v>
       </c>
       <c r="I28" t="s">
-        <v>144</v>
+        <v>182</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B29" t="s">
         <v>87</v>
       </c>
       <c r="C29" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="D29" t="s">
-        <v>145</v>
+        <v>107</v>
       </c>
       <c r="E29" t="s">
-        <v>146</v>
+        <v>108</v>
       </c>
       <c r="F29" t="s">
-        <v>147</v>
+        <v>109</v>
       </c>
       <c r="G29" t="s">
-        <v>148</v>
+        <v>110</v>
       </c>
       <c r="H29" t="s">
-        <v>149</v>
+        <v>111</v>
       </c>
       <c r="I29" t="s">
-        <v>148</v>
+        <v>109</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B30" t="s">
         <v>87</v>
       </c>
       <c r="C30" t="s">
-        <v>124</v>
+        <v>106</v>
       </c>
       <c r="D30" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="E30" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="F30" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="G30" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="H30" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="I30" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
@@ -2280,94 +2280,94 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="B32" t="s">
         <v>87</v>
       </c>
       <c r="C32" t="s">
-        <v>124</v>
+        <v>94</v>
       </c>
       <c r="D32" t="s">
-        <v>160</v>
+        <v>95</v>
       </c>
       <c r="E32" t="s">
-        <v>161</v>
+        <v>96</v>
       </c>
       <c r="F32" t="s">
-        <v>162</v>
+        <v>97</v>
       </c>
       <c r="G32" t="s">
-        <v>163</v>
+        <v>98</v>
       </c>
       <c r="H32" t="s">
-        <v>164</v>
+        <v>99</v>
       </c>
       <c r="I32" t="s">
-        <v>164</v>
+        <v>99</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="B33" t="s">
         <v>87</v>
       </c>
       <c r="C33" t="s">
-        <v>124</v>
+        <v>100</v>
       </c>
       <c r="D33" t="s">
-        <v>165</v>
+        <v>145</v>
       </c>
       <c r="E33" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
       <c r="F33" t="s">
-        <v>167</v>
+        <v>147</v>
       </c>
       <c r="G33" t="s">
-        <v>168</v>
+        <v>148</v>
       </c>
       <c r="H33" t="s">
-        <v>169</v>
+        <v>149</v>
       </c>
       <c r="I33" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="B34" t="s">
         <v>87</v>
       </c>
       <c r="C34" t="s">
-        <v>118</v>
+        <v>100</v>
       </c>
       <c r="D34" t="s">
-        <v>170</v>
+        <v>101</v>
       </c>
       <c r="E34" t="s">
-        <v>171</v>
+        <v>102</v>
       </c>
       <c r="F34" t="s">
-        <v>172</v>
+        <v>103</v>
       </c>
       <c r="G34" t="s">
-        <v>173</v>
+        <v>104</v>
       </c>
       <c r="H34" t="s">
-        <v>174</v>
+        <v>105</v>
       </c>
       <c r="I34" t="s">
-        <v>174</v>
+        <v>102</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B35" t="s">
         <v>87</v>
@@ -2376,54 +2376,58 @@
         <v>88</v>
       </c>
       <c r="D35" t="s">
-        <v>175</v>
+        <v>89</v>
       </c>
       <c r="E35" t="s">
-        <v>176</v>
+        <v>90</v>
       </c>
       <c r="F35" t="s">
-        <v>177</v>
+        <v>91</v>
       </c>
       <c r="G35" t="s">
-        <v>178</v>
+        <v>92</v>
       </c>
       <c r="H35" t="s">
-        <v>179</v>
+        <v>93</v>
       </c>
       <c r="I35" t="s">
-        <v>177</v>
+        <v>90</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B36" t="s">
         <v>87</v>
       </c>
       <c r="C36" t="s">
-        <v>112</v>
+        <v>88</v>
       </c>
       <c r="D36" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="E36" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="F36" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="G36" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="H36" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="I36" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:I36">
+    <sortCondition ref="B2:B36"/>
+    <sortCondition ref="A2:A36"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>